<commit_message>
UPDATE: README.md & minor fix
</commit_message>
<xml_diff>
--- a/output/radiko_190106/list乃木坂.xlsx
+++ b/output/radiko_190106/list乃木坂.xlsx
@@ -2048,6 +2048,24 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">

</xml_diff>